<commit_message>
update readme according feedback
</commit_message>
<xml_diff>
--- a/PerformanceData/fdtd_profile.xlsx
+++ b/PerformanceData/fdtd_profile.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tongw\Dropbox\assignments\CIS565_GPU\final\GPUVerb\GPUVerb\PerformanceData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8DB70994-26A9-426A-8D87-F18E92996B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B15D8F-F340-4E2B-8CDB-3E172C768932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1125" windowWidth="21600" windowHeight="13620"/>
+    <workbookView xWindow="6180" yWindow="1125" windowWidth="21600" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fdtd_profile" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -760,6 +760,15 @@
               <a:rPr lang="en-US" baseline="0"/>
               <a:t>GPU and CPU implementations</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>(Lower = Faster)</a:t>
+            </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
@@ -1495,7 +1504,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Dimension</a:t>
+                  <a:t> Dimension (Meters by Meters)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -2344,8 +2353,8 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>171449</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>147636</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
@@ -2675,11 +2684,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>